<commit_message>
Admin test cases functions By Mina
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_TC_Admin.xlsx
+++ b/Car_TestCases/Car_TC_Admin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>Test case ID</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>"Home" button shall be presented in admin home page and it shall be clickable and also shall navigate to "Add user" web page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1036,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C15:C16"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="89.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1525,6 +1528,9 @@
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
updates for Admin module test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_TC_Admin.xlsx
+++ b/Car_TestCases/Car_TC_Admin.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>Test case ID</t>
   </si>
@@ -63,97 +63,15 @@
 Password : lolo.lolo.123</t>
   </si>
   <si>
-    <t>Validate that the admin can login into the system using valid credentials</t>
-  </si>
-  <si>
-    <t>Car_SRS_32</t>
-  </si>
-  <si>
-    <t>The browser shall navigate to the admin home page</t>
-  </si>
-  <si>
     <t>Mina</t>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Car_SRS_33</t>
-  </si>
-  <si>
-    <t>Validate that the admin can add new user into the system</t>
   </si>
   <si>
     <t>Admin credentials 
 User Name : Admin123
 Password : lolo.lolo.124</t>
-  </si>
-  <si>
-    <t>Car_Add_Car_01 shall be passed</t>
-  </si>
-  <si>
-    <t>1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.</t>
-  </si>
-  <si>
-    <t>1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.
-5.The browser shall navigate to the admin home page.
-6.Press On " Add user " tab.
-7.The browser shall navigate to registration page.
-8.Fill in all field in the registration form using the given data.
-9.press On "register" button.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After a successful add user operation , The browser shall navigate to the admin home page again </t>
-  </si>
-  <si>
-    <t>Car_SRS_34</t>
-  </si>
-  <si>
-    <t>Admin account shall be exist
-any user account shall be exist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.
-5.The browser shall navigate to the admin home page.
-6.Press On " All users " tab.
-7.The browser shall navigate to all users page.
-8.Find Looza user account. 
-9.Press on 'delete user' tab.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-deleted user shall be removed also from all users pageand from users database table.</t>
-  </si>
-  <si>
-    <t>Car_SRS_35</t>
-  </si>
-  <si>
-    <t>Validate that the admin can delete existing user from the system</t>
-  </si>
-  <si>
-    <t>Validate that the admin can view existing users details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.
-5.The browser shall navigate to the admin home page.
-6.Press On " All users " tab.
-</t>
-  </si>
-  <si>
-    <t>All Users' information shall be displayed on the users page</t>
   </si>
   <si>
     <t>Car_Admin_01</t>
@@ -327,53 +245,12 @@
     <t>After a successful add car operation , The browser shall navigate to 'all car' page, and the new car shall be appeared in the page and shall be added to car database table.</t>
   </si>
   <si>
-    <t>Car_SRS_38</t>
-  </si>
-  <si>
     <t>Car_Admin_07</t>
   </si>
   <si>
-    <t>Validate that the admin can change car status from reserved to sold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin account shall be exist
-car which it's status will be changed, shall be exist </t>
-  </si>
-  <si>
     <t>Car_Admin_08</t>
   </si>
   <si>
-    <t>Car_SRS_39</t>
-  </si>
-  <si>
-    <t>Validate that the admin can change car status from reserved to free</t>
-  </si>
-  <si>
-    <t>the car status shall be changed to bought</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.
-5.The browser shall navigate to the admin home page.
-6.Press On " All Cars " tab.
-7.Find any car, and then from the drop down list which appears under the car photo, select 'free'
-8.refresh the current web page.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Launch the web browser
-2.go to the following URL : http://localhost/Car_implementation/ 
-3.Write the given admin Credentials in the user name and password text boxes.
-4.Press On the login button.
-5.The browser shall navigate to the admin home page.
-6.Press On " All Cars " tab.
-7.Find any car, and then from the drop down list which appears under the car photo, select bought
-8.refresh the current web page.
-</t>
-  </si>
-  <si>
     <t>Car_Admin_09</t>
   </si>
   <si>
@@ -384,55 +261,6 @@
   </si>
   <si>
     <t>Car_Admin_08 shall be executed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin credentials 
-User Name : Admin123
-Password : lolo.lolo.123
-New Account data 
-User Name : Looza 
-Email : Looza@gmail.com
-Address : Haram
-Phone : 012008009870
-Password : Looza2012
-</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Admin credentials </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-User Name : Admin123
-Password : lolo.lolo.123
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
   </si>
   <si>
     <r>
@@ -507,9 +335,6 @@
     <t>the reserved car shall not be found in the search page for users</t>
   </si>
   <si>
-    <t>the car status shall be changed to free and it shall be appeared for users in the search page</t>
-  </si>
-  <si>
     <t>Car_SRS_49</t>
   </si>
   <si>
@@ -517,15 +342,6 @@
   </si>
   <si>
     <t>Car_SRS_51</t>
-  </si>
-  <si>
-    <t>Car_Admin_11</t>
-  </si>
-  <si>
-    <t>Car_Admin_12</t>
-  </si>
-  <si>
-    <t>Car_Admin_13</t>
   </si>
   <si>
     <t xml:space="preserve">Validate that Admin home page shall contain "All Cars" button. </t>
@@ -558,9 +374,6 @@
     <t>"Reserved cars" button shall be presented in admin home page and it shall be clickable and also shall be navigate to "Reserved cars" web Page.</t>
   </si>
   <si>
-    <t>Car_Admin_14</t>
-  </si>
-  <si>
     <t>Admin credentials 
 User Name : Admin123
 Password : lolo.lolo.127</t>
@@ -569,9 +382,6 @@
     <t>UI&amp;Functional</t>
   </si>
   <si>
-    <t>Car_Admin_15</t>
-  </si>
-  <si>
     <t>Admin credentials 
 User Name : Admin123
 Password : lolo.lolo.128</t>
@@ -581,9 +391,6 @@
   </si>
   <si>
     <t>"Home" button shall be presented in admin home page and it shall be clickable and also shall navigate to "Home" web page</t>
-  </si>
-  <si>
-    <t>Car_Admin_16</t>
   </si>
   <si>
     <t>Validate that Admin home page shal contain " About Us"button</t>
@@ -690,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -702,9 +509,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1031,12 +835,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="89.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1091,492 +895,300 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="165.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="5" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>19</v>
+      <c r="D4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>29</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>19</v>
+      <c r="G9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="149.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
+      <c r="H10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="6" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="F11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="6" t="s">
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>